<commit_message>
Created csv to be imported into sql via phpmyadmin
Also created placeholder folders for web dev code.
</commit_message>
<xml_diff>
--- a/Relevant Spreadsheets/Drivers.xlsx
+++ b/Relevant Spreadsheets/Drivers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
   <si>
     <t>KIMI RÄIKKÖNEN</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>DRIVER NAME</t>
+  </si>
+  <si>
+    <t>''''''''''''''''''''''''''''''''''''</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -215,6 +218,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -527,13 +533,13 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>37</v>
@@ -555,13 +561,13 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="5">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>37</v>
@@ -569,13 +575,13 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="5">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>37</v>
@@ -597,27 +603,27 @@
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="5">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>37</v>
@@ -625,13 +631,13 @@
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="5">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>37</v>
@@ -639,13 +645,13 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="5">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>37</v>
@@ -653,44 +659,44 @@
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="5">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="5">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="5">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
@@ -709,159 +715,162 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="5">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="5">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1">
+    <row r="17" spans="1:5" ht="15" customHeight="1">
       <c r="A17" s="5">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="15" customHeight="1">
       <c r="A18" s="5">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="5">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="5">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1">
       <c r="A21" s="5">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="5">
+        <v>42</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1">
+      <c r="E22" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="5">
+        <v>44</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1">
+      <c r="A24" s="5">
+        <v>53</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1">
+      <c r="A25" s="5">
         <v>55</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1">
-      <c r="A24" s="5">
-        <v>33</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1">
-      <c r="A25" s="5">
-        <v>19</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="D25" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1">
+    <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="5">
         <v>77</v>
       </c>
@@ -875,21 +884,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1">
+    <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="A27" s="5">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1">
       <c r="C28" s="2"/>
       <c r="D28" s="5"/>
     </row>
@@ -916,8 +925,8 @@
       <c r="C47" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:C21">
-    <sortCondition ref="C2:C21"/>
+  <sortState ref="A2:D29">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>